<commit_message>
Final submission dashboard and integration
</commit_message>
<xml_diff>
--- a/BaseLocation.xlsx
+++ b/BaseLocation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="111">
   <si>
     <t>District_name</t>
   </si>
@@ -344,13 +344,16 @@
   </si>
   <si>
     <t>NEELANGARAI POLICE STATION</t>
+  </si>
+  <si>
+    <t>Mobile_Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +368,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -384,15 +397,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -684,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D104"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -695,9 +713,10 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,8 +729,11 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -724,8 +746,11 @@
       <c r="D2">
         <v>80.224270000000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>9693888954</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -738,8 +763,11 @@
       <c r="D3">
         <v>80.260869999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>9835214508</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -752,8 +780,11 @@
       <c r="D4">
         <v>80.273587000000006</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>9334335339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -766,8 +797,11 @@
       <c r="D5">
         <v>80.215773999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>8971709801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -780,8 +814,11 @@
       <c r="D6">
         <v>80.223063999999994</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>8294447787</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -794,8 +831,11 @@
       <c r="D7">
         <v>80.207779000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>8966324512</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -808,8 +848,11 @@
       <c r="D8">
         <v>80.286886999999993</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>9894715876</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -822,8 +865,11 @@
       <c r="D9">
         <v>80.225290000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>8971709213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -836,8 +882,11 @@
       <c r="D10">
         <v>80.278406000000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>9693888741</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -850,8 +899,11 @@
       <c r="D11">
         <v>80.249103000000005</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>8971702564</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -864,8 +916,11 @@
       <c r="D12">
         <v>80.285882000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>8845369871</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -878,8 +933,11 @@
       <c r="D13">
         <v>80.258071999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>9835456012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -892,8 +950,11 @@
       <c r="D14">
         <v>80.255865</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="2">
+        <v>9934164003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -906,8 +967,11 @@
       <c r="D15">
         <v>80.251621999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="2">
+        <v>9934164004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -920,8 +984,11 @@
       <c r="D16">
         <v>80.258539999999996</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="2">
+        <v>9934164005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -934,8 +1001,11 @@
       <c r="D17">
         <v>80.187351000000007</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="2">
+        <v>9934164027</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -948,8 +1018,11 @@
       <c r="D18">
         <v>80.278445000000005</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="2">
+        <v>9934164032</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -962,8 +1035,11 @@
       <c r="D19">
         <v>80.240876999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>9216000081</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -976,8 +1052,11 @@
       <c r="D20">
         <v>80.230269000000007</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>9216001808</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -990,8 +1069,11 @@
       <c r="D21">
         <v>80.218452999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>9216001859</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1004,8 +1086,11 @@
       <c r="D22">
         <v>80.223571000000007</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>9216103705</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1018,8 +1103,11 @@
       <c r="D23">
         <v>80.209654</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>9755974116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1032,8 +1120,11 @@
       <c r="D24">
         <v>80.275052000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>9755858671</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1046,8 +1137,11 @@
       <c r="D25">
         <v>80.263892999999996</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>9755759990</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1060,8 +1154,11 @@
       <c r="D26">
         <v>80.219239999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>9755369104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1074,8 +1171,11 @@
       <c r="D27">
         <v>80.242514999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>9993558512</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1088,8 +1188,11 @@
       <c r="D28">
         <v>80.276196999999996</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>9993558523</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1102,8 +1205,11 @@
       <c r="D29">
         <v>80.229481000000007</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>9993559112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1116,8 +1222,11 @@
       <c r="D30">
         <v>80.237527999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>9993558365</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1130,8 +1239,11 @@
       <c r="D31">
         <v>80.154915000000003</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>9993559074</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1144,8 +1256,11 @@
       <c r="D32">
         <v>80.061914999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" s="3">
+        <v>9899570762</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1158,8 +1273,11 @@
       <c r="D33">
         <v>80.097677000000004</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" s="3">
+        <v>9899570764</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1172,8 +1290,11 @@
       <c r="D34">
         <v>79.760659000000004</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" s="3">
+        <v>9899570808</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1186,8 +1307,11 @@
       <c r="D35">
         <v>79.817221000000004</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" s="3">
+        <v>9899570813</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1200,8 +1324,11 @@
       <c r="D36">
         <v>80.202772999999993</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <v>9825269655</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1214,8 +1341,11 @@
       <c r="D37">
         <v>79.614176</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>9824060573</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -1228,8 +1358,11 @@
       <c r="D38">
         <v>79.686387999999994</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>9825865168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -1242,8 +1375,11 @@
       <c r="D39">
         <v>79.709855000000005</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>9825022295</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1256,8 +1392,11 @@
       <c r="D40">
         <v>79.709760000000003</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>9824050801</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -1270,8 +1409,11 @@
       <c r="D41">
         <v>80.021642999999997</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" s="2">
+        <v>9898300015</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -1284,8 +1426,11 @@
       <c r="D42">
         <v>80.118104000000002</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" s="2">
+        <v>9898300028</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -1298,8 +1443,11 @@
       <c r="D43">
         <v>79.816909999999993</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" s="2">
+        <v>9898300040</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -1312,8 +1460,11 @@
       <c r="D44">
         <v>79.979482000000004</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" s="2">
+        <v>9898300041</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -1326,8 +1477,11 @@
       <c r="D45">
         <v>80.006429999999995</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45">
+        <v>9210659890</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -1340,8 +1494,11 @@
       <c r="D46">
         <v>80.025733000000002</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46">
+        <v>9213244346</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -1354,8 +1511,11 @@
       <c r="D47">
         <v>80.220445999999995</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47">
+        <v>9213244678</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -1368,8 +1528,11 @@
       <c r="D48">
         <v>79.980298000000005</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48">
+        <v>9213359351</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -1382,8 +1545,11 @@
       <c r="D49">
         <v>79.890119999999996</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49">
+        <v>9213222830</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -1396,8 +1562,11 @@
       <c r="D50">
         <v>80.231701000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50">
+        <v>9213820352</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -1410,8 +1579,11 @@
       <c r="D51">
         <v>80.104183000000006</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51">
+        <v>9213352603</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>34</v>
       </c>
@@ -1424,8 +1596,11 @@
       <c r="D52">
         <v>79.944255999999996</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52">
+        <v>9210306856</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -1438,8 +1613,11 @@
       <c r="D53">
         <v>80.107515000000006</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53">
+        <v>9210458065</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>34</v>
       </c>
@@ -1452,8 +1630,11 @@
       <c r="D54">
         <v>79.702331999999998</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54">
+        <v>9210452310</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>34</v>
       </c>
@@ -1466,8 +1647,11 @@
       <c r="D55">
         <v>80.058646999999993</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55">
+        <v>9210580412</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -1480,8 +1664,11 @@
       <c r="D56">
         <v>79.703052999999997</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56">
+        <v>9213601721</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -1494,8 +1681,11 @@
       <c r="D57">
         <v>80.134293999999997</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" s="2">
+        <v>9827700015</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -1508,8 +1698,11 @@
       <c r="D58">
         <v>79.832717000000002</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58" s="2">
+        <v>9827700092</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -1522,8 +1715,11 @@
       <c r="D59">
         <v>80.152280000000005</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59" s="2">
+        <v>9827708219</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>34</v>
       </c>
@@ -1536,8 +1732,11 @@
       <c r="D60">
         <v>80.180871999999994</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60" s="2">
+        <v>9827708258</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -1550,8 +1749,11 @@
       <c r="D61">
         <v>79.754219000000006</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61" s="2">
+        <v>9827708269</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -1564,8 +1766,11 @@
       <c r="D62">
         <v>79.980298000000005</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62" s="4">
+        <v>9444307544</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>34</v>
       </c>
@@ -1578,8 +1783,11 @@
       <c r="D63">
         <v>79.762636000000001</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63" s="4">
+        <v>9841184725</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -1592,8 +1800,11 @@
       <c r="D64">
         <v>80.002639000000002</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64" s="4">
+        <v>9444032428</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -1606,8 +1817,11 @@
       <c r="D65">
         <v>80.192513000000005</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65" s="4">
+        <v>9841518221</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>34</v>
       </c>
@@ -1620,8 +1834,11 @@
       <c r="D66">
         <v>80.210862000000006</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66" s="4">
+        <v>9840231471</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -1634,8 +1851,11 @@
       <c r="D67">
         <v>80.123456000000004</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67" s="3">
+        <v>9899570808</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>34</v>
       </c>
@@ -1648,8 +1868,11 @@
       <c r="D68">
         <v>80.226271999999994</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68" s="3">
+        <v>9899570813</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -1662,8 +1885,11 @@
       <c r="D69">
         <v>80.001802999999995</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69">
+        <v>9825269655</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>34</v>
       </c>
@@ -1676,8 +1902,11 @@
       <c r="D70">
         <v>79.671059999999997</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70">
+        <v>9824060573</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>34</v>
       </c>
@@ -1690,8 +1919,11 @@
       <c r="D71">
         <v>79.906170000000003</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71">
+        <v>9825865168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>34</v>
       </c>
@@ -1704,8 +1936,11 @@
       <c r="D72">
         <v>80.249403000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72">
+        <v>9825022295</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -1718,8 +1953,11 @@
       <c r="D73">
         <v>80.197445999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73">
+        <v>9824050801</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>70</v>
       </c>
@@ -1732,8 +1970,11 @@
       <c r="D74">
         <v>79.911139000000006</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74" s="2">
+        <v>9898300015</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>70</v>
       </c>
@@ -1746,8 +1987,11 @@
       <c r="D75">
         <v>80.020273000000003</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75" s="2">
+        <v>9898300028</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -1760,8 +2004,11 @@
       <c r="D76">
         <v>79.502021999999997</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76" s="2">
+        <v>9898300040</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>70</v>
       </c>
@@ -1774,8 +2021,11 @@
       <c r="D77">
         <v>80.183994999999996</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77" s="2">
+        <v>9898300041</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>70</v>
       </c>
@@ -1788,8 +2038,11 @@
       <c r="D78">
         <v>80.081489000000005</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78">
+        <v>9210659890</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>70</v>
       </c>
@@ -1802,8 +2055,11 @@
       <c r="D79">
         <v>79.614341999999994</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79">
+        <v>9213244346</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>70</v>
       </c>
@@ -1816,8 +2072,11 @@
       <c r="D80">
         <v>80.182682999999997</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="E80">
+        <v>9213244678</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>70</v>
       </c>
@@ -1830,8 +2089,11 @@
       <c r="D81">
         <v>79.853363999999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="E81">
+        <v>9213359351</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>70</v>
       </c>
@@ -1844,8 +2106,11 @@
       <c r="D82">
         <v>80.043098000000001</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="E82">
+        <v>8971709801</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>70</v>
       </c>
@@ -1858,8 +2123,11 @@
       <c r="D83">
         <v>80.138498999999996</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="E83">
+        <v>8294447787</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>70</v>
       </c>
@@ -1872,8 +2140,11 @@
       <c r="D84">
         <v>80.169948000000005</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="E84">
+        <v>8966324512</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>70</v>
       </c>
@@ -1886,8 +2157,11 @@
       <c r="D85">
         <v>80.202121000000005</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="E85">
+        <v>9894715876</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>70</v>
       </c>
@@ -1900,8 +2174,11 @@
       <c r="D86">
         <v>80.313849000000005</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="E86">
+        <v>8971709213</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>70</v>
       </c>
@@ -1914,8 +2191,11 @@
       <c r="D87">
         <v>80.107246000000004</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="E87">
+        <v>9693888741</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>70</v>
       </c>
@@ -1928,8 +2208,11 @@
       <c r="D88">
         <v>79.48433</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="E88">
+        <v>8971702564</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>70</v>
       </c>
@@ -1942,8 +2225,11 @@
       <c r="D89">
         <v>79.896709000000001</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="E89">
+        <v>8845369871</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>70</v>
       </c>
@@ -1956,8 +2242,11 @@
       <c r="D90">
         <v>79.910832999999997</v>
       </c>
-    </row>
-    <row r="91" spans="1:4">
+      <c r="E90">
+        <v>9835456012</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>70</v>
       </c>
@@ -1970,8 +2259,11 @@
       <c r="D91">
         <v>80.173040999999998</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="E91" s="2">
+        <v>9934164003</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>70</v>
       </c>
@@ -1984,8 +2276,11 @@
       <c r="D92">
         <v>80.129895000000005</v>
       </c>
-    </row>
-    <row r="93" spans="1:4">
+      <c r="E92" s="2">
+        <v>9934164004</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>70</v>
       </c>
@@ -1998,8 +2293,11 @@
       <c r="D93">
         <v>80.219620000000006</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="E93" s="2">
+        <v>9934164005</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>70</v>
       </c>
@@ -2012,8 +2310,11 @@
       <c r="D94">
         <v>79.756185000000002</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="E94" s="2">
+        <v>9934164027</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>70</v>
       </c>
@@ -2026,8 +2327,11 @@
       <c r="D95">
         <v>80.029697999999996</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="E95" s="2">
+        <v>9934164032</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>70</v>
       </c>
@@ -2040,8 +2344,11 @@
       <c r="D96">
         <v>79.619850999999997</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="E96">
+        <v>9216001808</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>70</v>
       </c>
@@ -2054,8 +2361,11 @@
       <c r="D97">
         <v>80.152778999999995</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="E97">
+        <v>9216001859</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>70</v>
       </c>
@@ -2068,8 +2378,11 @@
       <c r="D98">
         <v>80.261004</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="E98">
+        <v>9216103705</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>70</v>
       </c>
@@ -2082,8 +2395,11 @@
       <c r="D99">
         <v>79.860955000000004</v>
       </c>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="E99">
+        <v>9755974116</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>70</v>
       </c>
@@ -2096,8 +2412,11 @@
       <c r="D100">
         <v>79.898227000000006</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
+      <c r="E100">
+        <v>9755858671</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>70</v>
       </c>
@@ -2110,8 +2429,11 @@
       <c r="D101">
         <v>80.320031</v>
       </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="E101">
+        <v>9755759990</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>70</v>
       </c>
@@ -2124,8 +2446,11 @@
       <c r="D102">
         <v>80.098025000000007</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="E102">
+        <v>9755369104</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>70</v>
       </c>
@@ -2138,8 +2463,11 @@
       <c r="D103">
         <v>79.911021000000005</v>
       </c>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="E103">
+        <v>9993558512</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>70</v>
       </c>
@@ -2151,6 +2479,9 @@
       </c>
       <c r="D104">
         <v>80.166321999999994</v>
+      </c>
+      <c r="E104">
+        <v>9993558523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>